<commit_message>
pre-game update, -6 days
</commit_message>
<xml_diff>
--- a/out_there/mielet.xlsx
+++ b/out_there/mielet.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dare/posthuman-text/out_there/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0ACD47A-FD47-734E-BAFA-E0752AAB48DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="460" windowWidth="25600" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="444">
   <si>
     <t>#</t>
   </si>
@@ -1308,9 +1302,6 @@
     <t>labrateknikko</t>
   </si>
   <si>
-    <t>taiteien opiskelija</t>
-  </si>
-  <si>
     <t>Gabriela Indemar</t>
   </si>
   <si>
@@ -1335,17 +1326,38 @@
     <t>Taman Sari</t>
   </si>
   <si>
-    <t>korkean paikan hitsaaja</t>
-  </si>
-  <si>
     <t>mekaniikka</t>
+  </si>
+  <si>
+    <t>Fajar Setiawan</t>
+  </si>
+  <si>
+    <t>musiikin opiskelija</t>
+  </si>
+  <si>
+    <t>musiikki</t>
+  </si>
+  <si>
+    <t>löytää paikkansa maailmassa</t>
+  </si>
+  <si>
+    <t>Dravid Klumm</t>
+  </si>
+  <si>
+    <t>labrapäällikkö / Pikiran</t>
+  </si>
+  <si>
+    <t>laboratoriotekniikka</t>
+  </si>
+  <si>
+    <t>huoltoteknikko / Pikiran</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1437,7 +1449,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1464,6 +1476,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1476,7 +1490,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="17" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="28">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1493,6 +1507,8 @@
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1838,15 +1854,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q107"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K107" sqref="K107"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="3" customWidth="1"/>
@@ -1861,7 +1877,7 @@
     <col min="15" max="15" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2712,7 +2728,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" ht="15">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2749,7 +2765,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" ht="15">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2780,7 +2796,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" ht="15">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2814,7 +2830,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" ht="15">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2848,7 +2864,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" ht="15">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -3052,7 +3068,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" ht="15">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -3092,7 +3108,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" ht="15">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -3163,7 +3179,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" ht="15">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -3379,7 +3395,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" ht="15">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -3496,7 +3512,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" ht="15">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3530,7 +3546,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" ht="15">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3564,7 +3580,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" ht="15">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3595,7 +3611,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" ht="15">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3635,7 +3651,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" ht="15">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3672,7 +3688,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" ht="15">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -3743,7 +3759,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" ht="15">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -3786,7 +3802,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" ht="15">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -3854,7 +3870,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" ht="15">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -3931,7 +3947,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" ht="15">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -4042,7 +4058,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" ht="15">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -4079,7 +4095,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" ht="15">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -4155,7 +4171,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" ht="15">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -4229,7 +4245,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" ht="15">
       <c r="A67">
         <f t="shared" ref="A67:A101" si="2">ROW()-1</f>
         <v>66</v>
@@ -4247,7 +4263,7 @@
         <v>2113</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F104" si="3">(2133-E67)</f>
+        <f t="shared" ref="F67:F105" si="3">(2133-E67)</f>
         <v>20</v>
       </c>
       <c r="G67" s="2">
@@ -4265,7 +4281,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" ht="15">
       <c r="A68">
         <f t="shared" si="2"/>
         <v>67</v>
@@ -4299,7 +4315,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" ht="15">
       <c r="A69">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -4409,7 +4425,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" ht="15">
       <c r="A72">
         <f t="shared" si="2"/>
         <v>71</v>
@@ -4553,7 +4569,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" ht="15">
       <c r="A76">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -4587,7 +4603,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" ht="15">
       <c r="A77">
         <f t="shared" si="2"/>
         <v>76</v>
@@ -4626,7 +4642,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" ht="15">
       <c r="A78">
         <f t="shared" si="2"/>
         <v>77</v>
@@ -4663,7 +4679,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" ht="15">
       <c r="A79">
         <f t="shared" si="2"/>
         <v>78</v>
@@ -4697,7 +4713,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" ht="15">
       <c r="A80">
         <f t="shared" si="2"/>
         <v>79</v>
@@ -4731,7 +4747,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" ht="15">
       <c r="A81">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -4839,7 +4855,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" ht="15">
       <c r="A84">
         <f t="shared" si="2"/>
         <v>83</v>
@@ -4873,7 +4889,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" ht="15">
       <c r="A85">
         <f t="shared" si="2"/>
         <v>84</v>
@@ -4909,7 +4925,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" ht="15">
       <c r="A86">
         <f t="shared" si="2"/>
         <v>85</v>
@@ -4977,7 +4993,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" ht="15">
       <c r="A88">
         <f t="shared" si="2"/>
         <v>87</v>
@@ -5079,7 +5095,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" ht="15">
       <c r="A91">
         <f t="shared" si="2"/>
         <v>90</v>
@@ -5184,7 +5200,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" ht="15">
       <c r="A94">
         <f t="shared" si="2"/>
         <v>93</v>
@@ -5255,7 +5271,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" ht="15">
       <c r="A96">
         <f t="shared" si="2"/>
         <v>95</v>
@@ -5289,7 +5305,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" ht="15">
       <c r="A97">
         <f t="shared" si="2"/>
         <v>96</v>
@@ -5326,7 +5342,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" ht="15">
       <c r="A98">
         <f t="shared" si="2"/>
         <v>97</v>
@@ -5403,7 +5419,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" ht="15">
       <c r="A100">
         <f t="shared" si="2"/>
         <v>99</v>
@@ -5553,7 +5569,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C104" t="s">
         <v>426</v>
@@ -5581,18 +5597,43 @@
         <v>1</v>
       </c>
       <c r="N104" t="s">
+        <v>432</v>
+      </c>
+      <c r="O104" t="s">
         <v>433</v>
-      </c>
-      <c r="O104" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="105" spans="1:15">
       <c r="A105">
         <v>104</v>
       </c>
+      <c r="B105" s="3" t="s">
+        <v>436</v>
+      </c>
       <c r="C105" t="s">
-        <v>427</v>
+        <v>437</v>
+      </c>
+      <c r="D105" t="s">
+        <v>10</v>
+      </c>
+      <c r="E105">
+        <v>2110</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="G105" s="2">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>1</v>
+      </c>
+      <c r="N105" t="s">
+        <v>438</v>
+      </c>
+      <c r="O105" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="106" spans="1:15">
@@ -5600,19 +5641,19 @@
         <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C106" t="s">
         <v>220</v>
       </c>
       <c r="D106" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E106">
         <v>2107</v>
       </c>
       <c r="F106">
-        <f t="shared" ref="F106:F107" si="4">(2133-E106)</f>
+        <f t="shared" ref="F106:F108" si="4">(2133-E106)</f>
         <v>26</v>
       </c>
       <c r="G106" s="2">
@@ -5622,10 +5663,10 @@
         <v>1</v>
       </c>
       <c r="N106" t="s">
+        <v>429</v>
+      </c>
+      <c r="O106" t="s">
         <v>430</v>
-      </c>
-      <c r="O106" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="107" spans="1:15">
@@ -5633,10 +5674,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C107" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="D107" t="s">
         <v>10</v>
@@ -5655,61 +5696,91 @@
         <v>1</v>
       </c>
       <c r="N107" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="O107" t="s">
         <v>406</v>
       </c>
     </row>
+    <row r="108" spans="1:15">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="C108" t="s">
+        <v>441</v>
+      </c>
+      <c r="D108" t="s">
+        <v>51</v>
+      </c>
+      <c r="E108">
+        <v>2100</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="G108" s="2">
+        <v>1</v>
+      </c>
+      <c r="N108" t="s">
+        <v>442</v>
+      </c>
+      <c r="O108" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" location="vanesa-novitasari" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B7" r:id="rId2" location="gamanto-prasetyo" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B13" r:id="rId3" location="dinda-kusmawati" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B16" r:id="rId4" location="purwa-thamrin" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B18" r:id="rId5" location="rachel-novitasari" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B25" r:id="rId6" location="kuncara-hidayanto" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B26" r:id="rId7" location="bakda-gunarto" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B27" r:id="rId8" location="laksana-hidayat" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B28" r:id="rId9" location="dono-sitorus" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B29" r:id="rId10" location="diana-laksmiwati" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B91" r:id="rId11" location="gading-mangunsong" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B76" r:id="rId12" location="lantar-putra" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B96" r:id="rId13" location="zulaikha-namaga" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B100" r:id="rId14" location="tania-aryani" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B80" r:id="rId15" location="keisha-andriani" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B47" r:id="rId16" location="nyoman-saragih" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B48" r:id="rId17" location="marsudi-sihotang" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B49" r:id="rId18" location="wulan-pertiwi" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B50" r:id="rId19" location="faizah-anggraini" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B51" r:id="rId20" location="zulaikha-widiastuti" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B55" r:id="rId21" location="mahmud-nashiruddin" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B84" r:id="rId22" location="lidya-winarsih" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B88" r:id="rId23" location="lidya-utami" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B44" r:id="rId24" location="hartaka-situmorang" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B68" r:id="rId25" location="agus-habibi" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B78" r:id="rId26" location="agus-habibi" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B35" r:id="rId27" location="daruna-saragih" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B85" r:id="rId28" location="ozy-nugroho" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B86" r:id="rId29" location="alambana-sirait" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B97" r:id="rId30" location="lili-nurdiyanti" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B94" r:id="rId31" location="putu-ramadan" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B38" r:id="rId32" location="raina-wahyuni" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B62" r:id="rId33" location="atma-hutasoit" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B54" r:id="rId34" location="ibrahim-mustofa" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B72" r:id="rId35" location="ulva-mayasari" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B81" r:id="rId36" location="artanto-kurniawan" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B63" r:id="rId37" location="garda-wasita" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B79" r:id="rId38" location="lalita-pertiwi" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B59" r:id="rId39" location="himawan-maryadi" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B77" r:id="rId40" location="yani-pudjiastuti" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B36" r:id="rId41" location="umar-ramadan" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B98" r:id="rId42" location="mariadi-hutagalung" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B52" r:id="rId43" location="diana-farida" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B57" r:id="rId44" location="dipa-halim" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B65" r:id="rId45" location="dartono-samosir" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B67" r:id="rId46" location="rahmi-nasyiah" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B69" r:id="rId47" location="ina-melani" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B17" r:id="rId1" location="vanesa-novitasari"/>
+    <hyperlink ref="B7" r:id="rId2" location="gamanto-prasetyo"/>
+    <hyperlink ref="B13" r:id="rId3" location="dinda-kusmawati"/>
+    <hyperlink ref="B16" r:id="rId4" location="purwa-thamrin"/>
+    <hyperlink ref="B18" r:id="rId5" location="rachel-novitasari"/>
+    <hyperlink ref="B25" r:id="rId6" location="kuncara-hidayanto"/>
+    <hyperlink ref="B26" r:id="rId7" location="bakda-gunarto"/>
+    <hyperlink ref="B27" r:id="rId8" location="laksana-hidayat"/>
+    <hyperlink ref="B28" r:id="rId9" location="dono-sitorus"/>
+    <hyperlink ref="B29" r:id="rId10" location="diana-laksmiwati"/>
+    <hyperlink ref="B91" r:id="rId11" location="gading-mangunsong"/>
+    <hyperlink ref="B76" r:id="rId12" location="lantar-putra"/>
+    <hyperlink ref="B96" r:id="rId13" location="zulaikha-namaga"/>
+    <hyperlink ref="B100" r:id="rId14" location="tania-aryani"/>
+    <hyperlink ref="B80" r:id="rId15" location="keisha-andriani"/>
+    <hyperlink ref="B47" r:id="rId16" location="nyoman-saragih"/>
+    <hyperlink ref="B48" r:id="rId17" location="marsudi-sihotang"/>
+    <hyperlink ref="B49" r:id="rId18" location="wulan-pertiwi"/>
+    <hyperlink ref="B50" r:id="rId19" location="faizah-anggraini"/>
+    <hyperlink ref="B51" r:id="rId20" location="zulaikha-widiastuti"/>
+    <hyperlink ref="B55" r:id="rId21" location="mahmud-nashiruddin"/>
+    <hyperlink ref="B84" r:id="rId22" location="lidya-winarsih"/>
+    <hyperlink ref="B88" r:id="rId23" location="lidya-utami"/>
+    <hyperlink ref="B44" r:id="rId24" location="hartaka-situmorang"/>
+    <hyperlink ref="B68" r:id="rId25" location="agus-habibi"/>
+    <hyperlink ref="B78" r:id="rId26" location="agus-habibi"/>
+    <hyperlink ref="B35" r:id="rId27" location="daruna-saragih"/>
+    <hyperlink ref="B85" r:id="rId28" location="ozy-nugroho"/>
+    <hyperlink ref="B86" r:id="rId29" location="alambana-sirait"/>
+    <hyperlink ref="B97" r:id="rId30" location="lili-nurdiyanti"/>
+    <hyperlink ref="B94" r:id="rId31" location="putu-ramadan"/>
+    <hyperlink ref="B38" r:id="rId32" location="raina-wahyuni"/>
+    <hyperlink ref="B62" r:id="rId33" location="atma-hutasoit"/>
+    <hyperlink ref="B54" r:id="rId34" location="ibrahim-mustofa"/>
+    <hyperlink ref="B72" r:id="rId35" location="ulva-mayasari"/>
+    <hyperlink ref="B81" r:id="rId36" location="artanto-kurniawan"/>
+    <hyperlink ref="B63" r:id="rId37" location="garda-wasita"/>
+    <hyperlink ref="B79" r:id="rId38" location="lalita-pertiwi"/>
+    <hyperlink ref="B59" r:id="rId39" location="himawan-maryadi"/>
+    <hyperlink ref="B77" r:id="rId40" location="yani-pudjiastuti"/>
+    <hyperlink ref="B36" r:id="rId41" location="umar-ramadan"/>
+    <hyperlink ref="B98" r:id="rId42" location="mariadi-hutagalung"/>
+    <hyperlink ref="B52" r:id="rId43" location="diana-farida"/>
+    <hyperlink ref="B57" r:id="rId44" location="dipa-halim"/>
+    <hyperlink ref="B65" r:id="rId45" location="dartono-samosir"/>
+    <hyperlink ref="B67" r:id="rId46" location="rahmi-nasyiah"/>
+    <hyperlink ref="B69" r:id="rId47" location="ina-melani"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Out There, Sirenum updates
</commit_message>
<xml_diff>
--- a/out_there/mielet.xlsx
+++ b/out_there/mielet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="3560" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Egot" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="478">
   <si>
     <t>#</t>
   </si>
@@ -1357,9 +1357,6 @@
     <t>Sijainti</t>
   </si>
   <si>
-    <t>WT, N cargo</t>
-  </si>
-  <si>
     <t>Ralph Howard</t>
   </si>
   <si>
@@ -1436,6 +1433,27 @@
   </si>
   <si>
     <t>Taistelubotti</t>
+  </si>
+  <si>
+    <t>Adi Rambuka</t>
+  </si>
+  <si>
+    <t>rahtiteknikko</t>
+  </si>
+  <si>
+    <t>robottimorfien kauko-ohjaus</t>
+  </si>
+  <si>
+    <t>perhe, rikastuminen</t>
+  </si>
+  <si>
+    <t>WT, crew</t>
+  </si>
+  <si>
+    <t>Laser alukseen</t>
+  </si>
+  <si>
+    <t>WT, C cargo</t>
   </si>
 </sst>
 </file>
@@ -1542,7 +1560,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1572,6 +1590,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1586,7 +1605,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1606,6 +1625,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1955,8 +1975,8 @@
   <dimension ref="A1:Q108"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J93" sqref="J93"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -5893,9 +5913,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -5963,7 +5983,7 @@
         <v>444</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -5972,10 +5992,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="C2" t="s">
         <v>446</v>
-      </c>
-      <c r="C2" t="s">
-        <v>447</v>
       </c>
       <c r="D2" t="s">
         <v>44</v>
@@ -5997,16 +6017,16 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="O2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="P2" t="s">
-        <v>445</v>
+        <v>477</v>
       </c>
       <c r="Q2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -6015,10 +6035,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D3" t="s">
         <v>44</v>
@@ -6040,16 +6060,16 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
+        <v>450</v>
+      </c>
+      <c r="O3" t="s">
         <v>451</v>
       </c>
-      <c r="O3" t="s">
-        <v>452</v>
-      </c>
       <c r="P3" t="s">
-        <v>445</v>
+        <v>477</v>
       </c>
       <c r="Q3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -6058,10 +6078,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D4" t="s">
         <v>44</v>
@@ -6083,16 +6103,16 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="O4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="P4" t="s">
-        <v>445</v>
+        <v>477</v>
       </c>
       <c r="Q4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -6101,10 +6121,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
@@ -6129,16 +6149,16 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
+        <v>456</v>
+      </c>
+      <c r="O5" t="s">
         <v>457</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>458</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>459</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -6147,13 +6167,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E6">
         <v>2086</v>
@@ -6172,16 +6192,16 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O6" t="s">
+        <v>467</v>
+      </c>
+      <c r="P6" t="s">
         <v>468</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>469</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -6190,13 +6210,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E7">
         <v>2083</v>
@@ -6208,20 +6228,23 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
       <c r="M7">
         <v>1</v>
       </c>
       <c r="N7" t="s">
+        <v>466</v>
+      </c>
+      <c r="O7" t="s">
         <v>467</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>468</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>469</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -6229,10 +6252,42 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>471</v>
+      </c>
+      <c r="C8" t="s">
+        <v>472</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>2109</v>
+      </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>2133</v>
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>473</v>
+      </c>
+      <c r="O8" t="s">
+        <v>474</v>
+      </c>
+      <c r="P8" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="9" spans="1:17">

</xml_diff>